<commit_message>
Added Duty Cycle code and tested 25% 50% and 75% DC
</commit_message>
<xml_diff>
--- a/OvenTests/100DutyCycleAndCooldown.xlsx
+++ b/OvenTests/100DutyCycleAndCooldown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlols\OneDrive\Desktop\Schoolwork\9. Small Sat Research Lab\SSRLReflowOven\OvenTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB7B96D-06E5-49F2-9D69-F2279B2FD5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49367DB4-071C-4FDA-B8AC-E5B766712A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8F2C33F5-2ADF-4928-9153-2B5091CE37E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Time</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>With Oven Door Open</t>
   </si>
 </sst>
 </file>
@@ -13333,10 +13336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EE9BA3-84B9-4095-BD88-138CACD4263C}">
-  <dimension ref="A1:N1132"/>
+  <dimension ref="A1:P1132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -13628,7 +13631,7 @@
         <v>278.75</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>8</v>
       </c>
@@ -13645,8 +13648,11 @@
       <c r="N17">
         <v>277.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="P17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>8.5</v>
       </c>
@@ -13664,7 +13670,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>9</v>
       </c>
@@ -13682,7 +13688,7 @@
         <v>275.75</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>9.5</v>
       </c>
@@ -13700,7 +13706,7 @@
         <v>274.75</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>10</v>
       </c>
@@ -13718,7 +13724,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>10.5</v>
       </c>
@@ -13736,7 +13742,7 @@
         <v>272.75</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>11</v>
       </c>
@@ -13754,7 +13760,7 @@
         <v>271.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>11.5</v>
       </c>
@@ -13772,7 +13778,7 @@
         <v>270.75</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>12</v>
       </c>
@@ -13790,7 +13796,7 @@
         <v>270.25</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>12.5</v>
       </c>
@@ -13808,7 +13814,7 @@
         <v>269.25</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>13</v>
       </c>
@@ -13826,7 +13832,7 @@
         <v>268.25</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>13.5</v>
       </c>
@@ -13844,7 +13850,7 @@
         <v>267.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>14</v>
       </c>
@@ -13862,7 +13868,7 @@
         <v>266.5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>14.5</v>
       </c>
@@ -13880,7 +13886,7 @@
         <v>265.5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>15</v>
       </c>
@@ -13898,7 +13904,7 @@
         <v>264.75</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>15.5</v>
       </c>

</xml_diff>

<commit_message>
Cleaned up code with functions; added datasets for 90% 40% and 60% DC
</commit_message>
<xml_diff>
--- a/OvenTests/100DutyCycleAndCooldown.xlsx
+++ b/OvenTests/100DutyCycleAndCooldown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlols\OneDrive\Desktop\Schoolwork\9. Small Sat Research Lab\SSRLReflowOven\OvenTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49367DB4-071C-4FDA-B8AC-E5B766712A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA507341-59B0-4C1A-B3FF-309F262A5853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8F2C33F5-2ADF-4928-9153-2B5091CE37E1}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1452" windowWidth="11520" windowHeight="5040" xr2:uid="{8F2C33F5-2ADF-4928-9153-2B5091CE37E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,6 +214,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.4692475940507434E-2"/>
+                  <c:y val="0.39514909594634007"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$681</c:f>
@@ -13338,8 +13388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EE9BA3-84B9-4095-BD88-138CACD4263C}">
   <dimension ref="A1:P1132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>